<commit_message>
Get daily reddit data: Tue May  6 08:13:07 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_11.xlsx
+++ b/data/collected_data/2025_05_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C502"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3423 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1kfyt1k</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>I always just have regular black nails. How can I enhance them?</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4u3fzsr84ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1kfy63v</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Found my perfect winter combo — too bad it’s May</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfy63v</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1kfxx6s</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Press on recommendations</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfxx6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1kfxpza</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Oils for nail growth</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfxpza/oils_for_nail_growth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1kfxpth</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>What’s this shadow around my nails and why aren’t they curved properly?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xytczk3mu3ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1kfxdf0</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Being violently yeeted back into the short-nails lifestyle 💔</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otjqsqueq3ze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1kfx4t9</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Toe nail situation help</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0dzu82en3ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1kfwcf5</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Should I start looking somewhere else?</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfwcf5/should_i_start_looking_somewhere_else/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1kfwra5</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Compatible lamps for Aprés</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfwra5/compatible_lamps_for_aprés/</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1kfwju3</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Best Efile / Nail Drill</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfwju3/best_efile_nail_drill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1kfvln2</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>My friends first time doing ombré</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cresfac063ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1kfvigg</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Seeking recommendations for supplies</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfvigg/seeking_recommendations_for_supplies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1kfv7t7</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Is this overkill for nail care? These are the three products I use for my nails and cuticles.</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ndfr4cc223ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1kfuyw5</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>White French tip - staining</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jx0msadlz2ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1kfut8w</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>First time cat eye. Sorta failed lol</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rv1qkay0y2ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1kfupra</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>What happened to my French tips?</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbqsye80x2ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1kfupu4</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>I love Cala press ons</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twh8t412x2ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1kfu5wq</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Birthday nails! ACNH inspired</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfu5wq</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1kfu3kq</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Beginner Builder Gel Mani Spring</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfu3kq</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1kfu3je</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Does everyone need to take gel nail breaks or am I doing something wrong?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfu3je/does_everyone_need_to_take_gel_nail_breaks_or_am/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1kftzkg</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Gaming with nails lol</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ghfej4a4q2ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1kftxi2</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Creativity 🖊️</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kftxi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1kftni7</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Carey nails 🤎</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iv1xrvmym2ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1kftcl2</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>New nail popped off after 2 days</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kftcl2/new_nail_popped_off_after_2_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1kft75i</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>need to show people that appreciate it</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kft75i</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1kft2h3</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>First time using press ons</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kft2h3</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1kft10m</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Minimalist spring flowers 🌸🌼</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kft10m</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1kfsy7e</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Fruit🍓Salad🥗Yummy Yummy✨💅🏻</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfsy7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1kfsnlp</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Painted my nails for the first time in about three years</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4356isxxd2ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1kfsgao</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>First art set with the 5xl’s</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfsgao</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1kfs8tr</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>nail biter to cute long nails!</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfs8tr</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1kfrsb4</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>How long does your press on nails last?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfrsb4/how_long_does_your_press_on_nails_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1kfrowb</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>I couldn’t stop thinking about this design, so here’s my contribution to this cute fishy trend 🎣</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfrowb</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1kfq5xq</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Cherry blossom inspired nails 🌸</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czr12926s1ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1kfrntr</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Sheer Nails</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfrntr</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1kfrn37</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Very hungry caterpillar 🐛🍇🍓🍅🍭</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfrn37</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1kfrm6l</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>This week's manicure</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfrm6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1kfqzen</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Nail shape help</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfqzen</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1kfqjgz</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>A set im proud of 💖</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfqjgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1kfqfgp</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Kirby ⭐️</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6ph3x2eu1ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1kfqdkb</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>I love my watermelon cat eye nails!</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dy4vialxt1ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1kfpqen</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Bubbles when painting my nails</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfpqen</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1kfplje</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>At home gel x nails help</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfplje/at_home_gel_x_nails_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1kfpf1m</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Best Gel X Glue?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vz1vcfyl1ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1kfpv6n</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>My first print set!</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6br83c3op1ze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1kfprk8</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>got acrylics for the first time - I feel like a pretty princess 💜</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/np5tg03uo1ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1kfpbuk</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Better quality dupe?</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uy0fgs28l1ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1kfovq9</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Just need to feel my feelings with folks who get it</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f54nligkh1ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1kfoqjc</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Set of fire, what do you think?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ozu994gg1ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1kflygr</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>How does this happen and how do I stop it?</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b55tvoezv0ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1kfmkul</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>space girl 🛸</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u426wgzf01ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1kfnngd</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>How do I fix this?</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fmz8wy381ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1kfnzt1</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>nail polish + strengthener/conditioner?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfnzt1/nail_polish_strengthenerconditioner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1kfnp7d</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Looking for cuticle oil rec</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfnp7d/looking_for_cuticle_oil_rec/</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1kfnhu8</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Failed attempt at a cat eye with cherry blossoms :/</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/074cjs3z61ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1kfngch</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Recently found some crackle nail polish-- safe to say I'm reliving my childhood</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nzg3gzjp61ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1kfnavj</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>pretty n pink 🎀🌺</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfnavj</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1kfmsrt</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>What nails would fit my hands that are elegant? Recs?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnws243221ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1kfmskk</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Felt Like Spring</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42uyid0121ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1kfmpza</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>The Best Magnetic GEL Polishes?</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfmpza/the_best_magnetic_gel_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1kfmijy</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>lavender dreams</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avfserqyz0ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1kfmavj</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Second attempt at doing my own nails</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5e1ukify0ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1kfkqyu</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Press on advice/Alda glue?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfkqyu/press_on_advicealda_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1kfla7o</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Question about fills</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfla7o/question_about_fills/</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1kfliku</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Here fishy fishy... In action!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfliku</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1kflhag</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Got my nails done!! So pretty</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kflhag</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1kfl8ka</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Nails from home</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfl8ka/nails_from_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1kfl7zv</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Gel redo</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfl7zv/gel_redo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1kfl2xe</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Beauty is in the details 💅😍</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfl2xe</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1kfkr8c</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Gel overlay - how often to fill?</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfkr8c/gel_overlay_how_often_to_fill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1kfkkut</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Some of my recent nails</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfkkut</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1kfjnjw</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>So happy to have NAILSS</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gtbese3pf0ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1kfi7w7</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Nail Inspo Recommendations</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfi7w7</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1kfirkh</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Anime Character Inspired Press On Nail Set</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfirkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1kfitnq</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Damaged nail beds</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfitnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1kfj6wb</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Golden Spring ✨🧡💐</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfj6wb</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1kfizsi</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>My baseline nude ✨🤎</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3vo9rqya0ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1kfihxx</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>BCB Lacquers - Where We're Going You Don't Need Roads</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfihxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1kfh576</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Balled out for once, how did it turn out?</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfh576</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1kfi9x0</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Press ons: Tips to avoid getting hair caught?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfi9x0/press_ons_tips_to_avoid_getting_hair_caught/</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1kfhxnr</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Always faithful to my manicure</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3aijplk30ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1kfgocu</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Fun and cute</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfgocu</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1kfgbrj</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>My stunning hand painted nails 🧡🤍💙</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pz1llukbszye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1kfhbkw</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Mercy (Oberwatch) Nail Art</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfhbkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1kfh9jc</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>When you let a 4yr old pick your nail color</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfh9jc</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1kfh8v1</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Why wipes instead of washing when doing nails at home</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfh8v1/why_wipes_instead_of_washing_when_doing_nails_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1kfh6l1</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Structured gel manicure versus biosculpture?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kfh6l1/structured_gel_manicure_versus_biosculpture/</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1kfgsdd</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Cinnamoroll Nails!</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfgsdd</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1kfgqpo</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Squoval or almond?</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfgqpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1kfgkkj</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>beach nails!</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfgkkj</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1kfghp2</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Want to grow mine out :(</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfghp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1kfgawb</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>May the 4th be with you</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfgawb</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1kfg2yc</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Obsessed 🦋🐰</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/419ppryjqzye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1kffz3h</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>My favourite set so far</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kffz3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1kffngo</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Not my usual style</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kffngo</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1kffkan</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Hopped on the ladybug trend!</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8ghrynvmzye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1kffipw</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Natural nails growth</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kffipw</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1kfff1f</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>unfaithful to any man, but never to my manicure 😂</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hab4e6ytlzye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1kf5b0m</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Hello! Can somebody tell me how I can heal my nails/cuticle? Also general nail care tips pls :)</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kf5b0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1kf7ot9</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Nails splitting like crazy despite using acetone free nailpolish remover and taking care of them.</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kf7ot9/nails_splitting_like_crazy_despite_using_acetone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1kfywsp</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>I was sleeping on this one! 🌅</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfywsp</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1kfxo3b</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Why did my nail start cracking like this and why won’t it stop?</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfxo3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1kfvxrz</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>A few messy Mooncat manis</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfvxrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1kfvknj</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>selena gomez did lavender chrome so i did lavender chrome</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfvknj</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1kfvat4</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Back to the Colour Cube</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfvat4</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1kftzc7</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Potion of the Ocean</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iqrhlzt1q2ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1kftj3q</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Mooncat Witchcraft?</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kftj3q/mooncat_witchcraft/</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1kfteuk</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Pretty sure it's just magic at this point</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oxak9hlrk2ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1kftc1k</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Fake Halo by Mooncat 😈😇🌈</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0wborae6k2ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1kfsjdq</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Did some mermaid bait on my shorties</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfsjdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1kfsgdp</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Bee's Knees Lacquer's I Choose the Bear</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nav2hqmab2ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1kfsaf0</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>BKL Herbalism</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfsaf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1kfs0d2</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Square or round</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljdtqed582ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1kfrleq</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>LynB Designs sale haul with swatches and comparisons</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfrleq</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1kfrh1i</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>May the 4th be with you - Mooncat Death Star</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2wc0sbk932ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1kfqfc5</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>How could I get my cuticles to have a change like this?</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x17ml21du1ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1kfq78s</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Dupe request: OPI Skull &amp; Glossbones</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jvrfcsgs1ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1kfpllm</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Diamond nails experiment</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfpllm</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1kfpjen</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Dam Polish Question</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kfpjen/dam_polish_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1kfp5wa</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>dreamiest combo 😍</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfp5wa</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1kfopy9</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Halo 👼🏼</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xq5hixebg1ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1kfjho0</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>BKL Owl Bear Club</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dq1eb0tie0ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1kfo5zq</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Terrifying Visage - BKL</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfo5zq</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1kfnsy5</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>ILNP Hallucinate</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfnsy5</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1kfnlc7</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Neutral, but add some shimmer</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om3m90ko71ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1kfn6vl</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Looking for a dupe of Essence Wow Cacao 26</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfn6vl</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1kfmzia</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>First Clionadh Haul!</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfid13mb31ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1kfmzae</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Cactus Makes Perfect🌵🌺</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfmzae</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1kfmy40</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Love this navy blue!</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4g7o8y131ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1kfmhu2</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Why does BKL archive so many of their magnetics? Are they ever available again?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kfmhu2/why_does_bkl_archive_so_many_of_their_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1kfmge5</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Photography tips please!!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfmge5</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1kfme1u</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>probably my favorite light blue in my collection</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfme1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1kfm6h2</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Revenge of the 5th</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7zm7mmq3x0ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1kfm6aa</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Purple to pink ombre nails</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfm6aa</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1kfm1go</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Clionadh Sale Skittle!</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfm1go</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1kfkltb</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>my commute entertainment for the day</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8h9nodybm0ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1kfkih9</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>battle of the iridescents ⚔️</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfkih9</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1kfkclq</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>I think I ruined my favorite orange 🍊 color</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfkclq</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1kfk16m</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>BKL Toil and Trouble</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1gmcxmyai0ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1kfjyn0</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Press on guidance</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kfjyn0/press_on_guidance/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1kfjvgr</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Confetti Cannon (PPU Apr ‘25) 🎊</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfjvgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1kfjqkl</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Tried</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0j3si16bg0ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1kfjmhd</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>First time jelly non-gel</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1quzy21hf0ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1kfj8ro</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Dupe of Bubble Bath</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kfj8ro/dupe_of_bubble_bath/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1kfj34n</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Witchcraft!</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2icrt6xhb0ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1kfiw3c</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>THE beach vacay polish</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfiw3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1kfisdb</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>If frogs had wings…</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apk0025j90ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1kfiq8k</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>From my Mooncat haul - Just Bitten</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfiq8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1kfiiq5</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>More evidence that they should be toppers</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4cqbfbo70ze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1kfigyb</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>BCB Lacquers - Where We're Going You Don't Need Roads</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfigyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1kfibpv</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>mooncat forbidden fruit</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jn79zdnb60ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1kfiavp</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>favourite sally hansen miracle gel colours?</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kfiavp/favourite_sally_hansen_miracle_gel_colours/</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1kfhlr8</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Slice of the Party (Apr 25 PPU)</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfhlr8</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1kfheqf</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Cracked - Boujee Emerald</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oyjs5psvzzye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1kfgplu</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>beginner trying very hard!</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/feljzp04vzye1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1kff38r</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Suggested Mooncat Appreciation Post</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kff38r/suggested_mooncat_appreciation_post/</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1kfeo18</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Matched my tumbler 😂</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfeo18</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1kfeipt</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Infinity ♾️</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfeipt</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1kfe0vb</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>First ever PPU order last month, in love</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6lij9ghpbzye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1kfdwhm</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Morgan Taylor Rhythm and bluea</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i83eaxj1bzye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1kfdlim</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Holo Taco- Born Ugly</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfdlim</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1kfddfv</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Farewell to the booger green</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfddfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1kfd6bh</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>ILNP Lily</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q1pgas6p5zye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1kfcr7h</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>no words, just appreciation 💜✨</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfcr7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1kfchn9</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Professional Product Recs</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kfchn9/professional_product_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1kfc1l3</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>If anyone was looking for something similar to DVN's "Cooties"</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfc1l3</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1kf24z5</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Builder gel keeps lifting</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kf24z5/builder_gel_keeps_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1kf9zvz</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Lisa Frank Nails 🌈</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fv01flvbfyye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1kf9ei9</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Australian Indie Skittle - Cosmic Polish &amp; Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p9lf3luh9yye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1kf95cn</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>An OPI classic for the Bank Holiday weekend.</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kf95cn</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1kf7uwc</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kf7uwc/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1kfz4r2</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Any dry marble enthusiasts out there?</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2lypih4d4ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1kfxmoo</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Bugs!</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ewkxhhjit3ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1kfw6x5</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Nail Art Inspiration Thread</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kfw6x5/nail_art_inspiration_thread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1kfvo83</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Linework</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0wfcpxr63ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1kftmr4</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Any Australian press on nail artists in here??</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kftmr4/any_australian_press_on_nail_artists_in_here/</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1kfrr8q</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>First art set with the 5xl’s</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfrr8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1kfrged</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>I can’t tell if I like these or not 😩</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfrged</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1kfrew9</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Beach Ready ☀️🌊🐚</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfrew9</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1kfpw48</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>New and wanting to learn</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfpw48</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1kfpqnz</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>2nd hand painted set, how I do?</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0zp67dmo1ze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1kfpq1m</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Made these a little while ago</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfpq1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1kfobc6</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Showing support for the Dallas Stars Hockey team</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfobc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1kfnvqo</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>My newest creation!</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zw1y6zbw91ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1kfn3v7</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xf7fr6j641ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1kfmfes</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Had to hop on the fishing lure boat</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfmfes</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1kfmdtm</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Just some lil press ons</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfmdtm</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1kflvxy</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Added tips to my bare nails. What do you think?</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wi0j29gv0ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1kfln22</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>sketching designs</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfln22</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1kfkz6o</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Snake Jade</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24xeaia0p0ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1kfksuy</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>I’m a new nail tech🩷</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfqszazon0ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1kfke8n</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Made these last night</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfke8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1kfjh2c</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Trying out croco print 🐊</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfjh2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1kfjbfl</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>limon</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4lueukr8d0ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1kfinzk</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Design ideas for nails based off the album "In Love and Death" by The Used?</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57chspyo80ze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1kfha3p</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>What is the best way for an absolute beginner to learn nail art? I can draw and I am kicking around the idea of becoming a nail tech, but have no idea where to start with nail art. Your information is appreciated!</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kfha3p/what_is_the_best_way_for_an_absolute_beginner_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1kfgkfh</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>What do we think of this set?</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ojd2z92uzye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1kfgjhc</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Fun and cute</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfgjhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1kfform</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>The girls are out to play</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vr0r0c0qnzye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1kfdarc</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Anyone else play this game as a kid? 🥹 I was trying some flash reactive polish and it immediately made me think of this 😂</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvah9p4n6zye1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1kfabpo</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Spring nails💚</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4x2k2kediyye1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed May  7 08:13:23 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_11.xlsx
+++ b/data/collected_data/2025_05_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C502"/>
+  <dimension ref="A1:C699"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8967,6 +8967,3355 @@
         </is>
       </c>
     </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1kgrjfd</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>What shape should I try next?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgrjfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1kgri9t</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Do my natural nails look healthy?</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgri9t/do_my_natural_nails_look_healthy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1kgrd7y</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>My new spring nails :3</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/elvjfmkj9bze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1kgrd5k</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>one of my recent freestyles 😍💙</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wu6a4hi9bze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1kgr4dt</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Iv been doing my own nails for months and I think this is the best so far</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3aer2rtd6bze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1kgqrmv</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Milky Biab, almond shape</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cp5gtjr22bze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1kgo0sh</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Nail Designs/Art!</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgo0sh</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1kgobdi</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>what i got vs the inspo (last pic is from rednote user 918978389) what should i ask for next time for this look??</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgobdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1kgo40q</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Do you see 🎀  Or  ✂️ ?</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6h0cccc8aze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1kgo34s</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>My Glow in the Dark+Magnetic Gel Set</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m33c0dw28aze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1kgnnqd</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Can i file my Gel X extensions at home??</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgnnqd/can_i_file_my_gel_x_extensions_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1kgn7qq</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Tea pot inspired design</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgn7qq</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1kgm6mm</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>First time getting my nails done as a guy</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqhakh3tp9ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1kgn3yd</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Why won’t my press ons stay on?</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgn3yd/why_wont_my_press_ons_stay_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1kgn00m</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>is wearing press-ons (almost) back to back okay?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgn00m/is_wearing_pressons_almost_back_to_back_okay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1kgmztq</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>I wanted something delicate but feminine at the same time... I think I loved the result 🎀🌸🩷</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebudnhlex9ze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1kgm94i</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Gel/Acrylic Allergy</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgm94i</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1kgltn7</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>These nails really challenged me</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgltn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1kgll2i</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Where my “nub” girlies at? 😭</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgll2i</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1kgm10a</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Nothing too fancy but they cute 💅</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g66i2wrco9ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1kgl1nw</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>this feels like a weird take on cat eye but i don’t hate it?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5otaay1cf9ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1kgl1cn</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0jbdz79f9ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1kgkdp4</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Trying rounded shape for the first time</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12yv2zod99ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1kgkc3v</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Press ons have changed my life</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgkc3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1kgkazd</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Shiny Pink Spring Nails</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgkazd</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1kgjde0</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Plant based press on nail tips?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgjde0/plant_based_press_on_nail_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1kgjbsz</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Salon messed up my nails</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcc8am0909ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1kgjnq4</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>the first set of gel nails i've ever done!!</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgjnq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1kgjyhn</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Builder gel gapping in the middle of the nail? Why? It happens usually in the middle, not the edges…</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhk8amzn59ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1kgj7uw</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Nails cracking so low, what to do?</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1cqr08bz8ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1kgj7qg</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Perfect color match 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgj7qg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1kgiuwn</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Wanting to properly grow my nails out, but they grow out funny. How do I fix raised nails after from biting them for so long?</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgiuwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1kgizyy</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Silver chrome</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgizyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1kgizr5</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>I do my nails... periodically</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgizr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1kgivq8</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Tips on taking decent vids and pics to really capture the true color shifts</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tgxo1c9fw8ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1kghj01</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>unique natural shape or medical issue? 💀</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kghj01</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1kgires</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>spring nails</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bnudrccfv8ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1kgihjp</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Does anyone notice the very subtle game reference?</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xopy61k5t8ze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1kgiavw</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Simple magical design.</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ys46d1pr8ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1kgi1d0</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Gyaru inspired set</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgi1d0</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1kghxoc</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Need Full Coverage Nail Tip Recommendations</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljzwopkso8ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1kghm2g</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Nail lady is *chefs kiss*</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kghm2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1kghj8o</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>My last works with gems for your nail ideas 🥹✨ what do you think about them?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kghj8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1kghj3u</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Going from BIAB to acrylic?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kghj3u/going_from_biab_to_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1kghiqg</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Like taking nails off?</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kghiqg/like_taking_nails_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1kggo8f</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Poyo! (Kirby nails by me)</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kggo8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1kggo7a</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>I love the marble effect 💅</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fn6z5i92f8ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1kggljy</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Intruding Neglected Nail</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rt9pcwqhe8ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1kgghr9</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>🤷‍♀️🤷‍♀️</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgghr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1kggau7</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Seeking chrome press on for clubbed thumbs</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/873xkua9c8ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1kggcxd</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>DIY polygel.</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3vytw1coc8ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1kggb53</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>What colour combo should I try next? 👩🏻‍🔬</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jr79678bc8ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1kgg5cz</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Strengthen nails</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgg5cz/strengthen_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1kgg1dj</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Did my own nails for the first time in months 💅 obsessed with this color!</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgg1dj</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1kgftpd</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>What shape is this?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qi8mu1ro88ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1kgfbuw</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Thoughts on this length/shape for me? Nail tech actually said it’s the limit for how long I should grow my natural nails!</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0kc6nx258ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1kgfadd</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Opi intelli gel vs regular gel color difference</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t11ufeur48ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1kgf6ph</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Lavender holo sparkle ✨️💜✨️💜</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcrme3d048ze1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1kgemaj</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>💙 Polished For Days Ghoulish 💜</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgemaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1kgedzd</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>I chose something more CALM AND DELICATE 🩷🌸 so that it can be suitable for any type of occasion</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rkz1vf69y7ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1kge3u1</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Upset nail</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kge3u1/upset_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1kgec7y</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>I chose to make this design but it doesn't seem to convince me completely 🫤 I don't know if it's the color or the format I chose (although I like the heart 💜)</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9sgxeqwx7ze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1kge9x1</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>When it comes to PINK, it's never enough 🌸🩷</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhf807igx7ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1kge6pf</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>I only did the semi-permanent one for fun, and because I had the polishes hahaha, I don't hate them anyway, I liked them</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kge6pf</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1kgdxoc</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Gel x with hard gel?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgdxoc/gel_x_with_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1kgcsx2</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Why is my nail doing this?</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgcsx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1kgdew5</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>What would you say is the theme for these nails?</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgdew5</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1kgd8hp</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Gel polish lifting</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tfvt6tiwp7ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1kgcv1p</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Sun and blue sky design done at my local salon</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgcv1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1kgcihb</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Help With Manicure Package for Wife</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgcihb/help_with_manicure_package_for_wife/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1kgcmko</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>On the hunt for Natural Chrome</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgcmko/on_the_hunt_for_natural_chrome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1kgcjj2</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Darn it! Not 48hrs and broke it!</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgcjj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1kgci01</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Cottage Core Nails</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgci01</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1kgcbdh</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>She prettyyy ✨💖</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2hoti87j7ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1kgc7md</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Suggestion for Gift for GF?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgc7md/suggestion_for_gift_for_gf/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1kgc397</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>suggested by a friend...</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6pckk7mh7ze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1kgbudw</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Getting nails done for the first time soon!</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgbudw/getting_nails_done_for_the_first_time_soon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1kgbnel</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Nervous to go to the nail salon</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgbnel/nervous_to_go_to_the_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1kgb361</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Which nail shape should I get? (Acrylic gel)</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9x81dsha7ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1kgba0h</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>My current Japanese gel manicure 🧡</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6i9oif0sb7ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1kgbfog</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Just a moment for my first summer set</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgbfog</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1kgbd0d</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>NAILFIE</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgbd0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1kgb9bz</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Too early for strawberry nails?</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ty0703qnb7ze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1kgb7tn</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Something simple .</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6mmx36db7ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1kgb21r</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Advice needed for crusty nails and cuticles</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgb21r</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1kgazle</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Narrow nail bed girlies.. what shape do you usually go for?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ec3m98fs97ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1kgakh9</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>New nails what do we think?!</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0l47i9gs67ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1kga638</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Ink on Powdered Gel Acrylic</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kga638/ink_on_powdered_gel_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1kgab5i</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Is it giving Barbie?!</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgab5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1kgaa4a</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Long square to teeny tiny oval lol</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ty4exieq47ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1kg9ydj</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Are these *too square*?</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg9ydj</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1kg9x4q</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>5 weeks of growth!</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/558d2zp627ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1kg9ifw</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg9ifw</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1kg9rji</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>acrylic almond cat eye holo chrome</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg9rji</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1kg9laa</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>How to remove press ons applied with stickers/tabs?</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tpap2lwz6ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1kg9fhz</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>I’ve narrowed it down to this list.</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kg9fhz/ive_narrowed_it_down_to_this_list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1kg99dg</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>OBSESSED (by Jocelyn at Get Nailed) 🤩</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg99dg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1kg7utg</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>I Don’t know about this color 🙃</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg7utg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1kg96bi</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>How do I soften my nails?</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kg96bi/how_do_i_soften_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1kg8z4j</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>This baby pink might be my favorite</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k60fbi2gv6ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1kgpeh3</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Teatime nails!</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgpeh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1kgoux0</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Phoenix swatch request - Omega Telepathy / X collection</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lilanrizfaze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1kgnweg</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Convince me</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgnweg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1kgnpzj</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Clionadh skittle! ✨️</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s98yftre4aze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1kgn0qi</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>My new absolute favorite - Moon Shine Mani's April PPU</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgn0qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1kglrkt</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Cadillacquer is becoming a favorite 🤩</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hrvxda2zl9ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1kgljrq</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Showstopper Shades</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kgljrq/showstopper_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1kglc0c</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Marketplace Haul!</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1i2v6yzh9ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1kgl19n</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>What colours do you love, but never see mentioned?</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kgl19n/what_colours_do_you_love_but_never_see_mentioned/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1kgknp4</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Someone better hold my wallet</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6an7oktb9ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1kgkj2m</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Glisten &amp; Glow vs KB Shimmer basecoats, glitter grabbers, and topcoats</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kgkj2m/glisten_glow_vs_kb_shimmer_basecoats_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1kgkfji</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Do you keep the boxes?</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vlv8k8yt99ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1kgjq4m</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Best primer/neutral color for clear press-on base?</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/293z985m39ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1kgjovq</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Enjoy The Fall? Sure Will!🍂</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgjovq</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1kgj87p</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Cirque High Line question</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgj87p</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1kgj5zu</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Playing around resulted in the swampy green of my dreams</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgj5zu</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1kgi9og</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Phoenix Rosalie</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udr4402gr8ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1kgh70q</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Pink, purple, and rainbow</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/td1r1xzyi8ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1kghuda</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Del Sol: Day Dreamer☀️</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgfs0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1kggmgp</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>[LynB Designs] Calypso’s Birthday</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kggmgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1kggc0z</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Lemon-BKL</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kggc0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1kgg3mk</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>I'm IP banned from Drunk Fairy Polishes, AMA</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgg3mk</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1kgfs7b</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Cuticula Fairycore Dupe Attempts ✨</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0rm3l54b88ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1kgfor4</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Can you help me find polishes that match weird descriptions I provide?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kgfor4/can_you_help_me_find_polishes_that_match_weird/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1kgenpa</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Trying to dupe from my collection!</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4kjwt6kz7ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1kgein8</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>💙 Polished For Days Ghoulish 💜</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgein8</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1kgdndw</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Painted my nails last night. Got to work tonight and was gifted a matching puzzle!</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vcuq5guys7ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1kgdf7v</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Iridescent, glowy blue!</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgdf7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1kgd6vz</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Alien-esque!</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjsi1cgkp7ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1kgd5c2</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Does my new nail shape look okay?</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgd5c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1kgcl4h</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Flower Child’s louder sister Constant State of Phlox</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eh2y3gr5l7ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1kgbsw1</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>China Glaze ‘Limbo Bimbo’ 🩷</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/av5ltk5if7ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1kgbp6v</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Nude, but make it velvet</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/giakk3efe7ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1kgbo0t</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>BeBio Lacquer comparison!</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgbo0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1kgbagx</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>can’t stop staring at these 💙</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgbagx</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1kgb5om</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Spring pastel recommendations please</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kgb5om/spring_pastel_recommendations_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1kgb375</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Why does ILNP have polishes whose average rating are higher than 5.0?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kgb375/why_does_ilnp_have_polishes_whose_average_rating/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1kgax9i</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>First time posting! Making the switch from gels to regular polish</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fv10vufb97ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1kgan3y</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>My take on May the 4th (on the 6th 😅)</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgan3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1kgakro</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Caught the Wind in a Kite of a Dreams</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xb9q9wlu67ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1kgakmb</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>An Oldie but a Goodie</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzw4takt67ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1kgahft</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Referral/ affiliate codes?</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kgahft/referral_affiliate_codes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1kgaf2j</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Help me dupe my favorite pink neon</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgaf2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1kga8ye</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>ILNP Flower Child + Essie Play Date</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9witaibi47ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1kga397</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Riding a Unicorn 🦄</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kga397</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1kg9uwk</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Accidentally bought a skittle in one from Bees Knees 🤣</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32l7gsqq17ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1kg9sx5</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Is this not just a regular white polish??</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg9sx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1kg9k3t</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Try not to stare at nails all day challenge - Level: Impossible</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c7pn3yulz6ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1kg8m6i</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>One year since I got my very first polish...here are some of my favourite manis!</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg8m6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1kg8ipg</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Where to start</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg8ipg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1kg8d8n</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Nail Polish Color suggestions - Formal Wedding Emerald Green Dress, Gold Accessories</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kg8d8n/nail_polish_color_suggestions_formal_wedding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1kg84cw</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>“your nails but better” shade? 💗</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kg84cw/your_nails_but_better_shade/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1kg841w</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Hey Deez Nails</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg841w</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1kg83zc</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Good vibes for my kiddo + their spring flower-themed nails</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg83zc</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1kg82bc</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Brand Recs</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg82bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1kg7pg3</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Birthday brat v. Pink pony club</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kg7pg3/birthday_brat_v_pink_pony_club/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1kg7fqn</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>I don't really like red on my nails, but these dark reds are so stunning</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg7fqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1kg7dop</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Magic Frog🪄✨🐸✨🪄</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zmfrjbi1k6ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1kg6z03</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>mooncat forbidden fruit on a rainy day</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg6z03</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1kg6qi3</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Dreamscape and a bird</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg6qi3</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1kg65ms</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Combo for even better Mermaid vibes</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg65ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1kg62ub</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Mooncat/Cirque/BKL sale + April PPU blue and purple skittle</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg62ub</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1kg61l8</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Turkeys Over TERFies! Silly mani for a serious purpose 🦃 🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/640j8z3ea6ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1kg5n1e</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>I’m really proud of how this Lisa Frank inspired mani turned out! 🌈🐬🐯</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg5n1e</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1kg4x7d</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Clover 🍀</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7oqsd3t16ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1kg4n8o</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>"The Evil Within / PsychoBreak 1" video game tribute nails</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg4n8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1kg49bk</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Star Wars galaxy nails</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qw5kq0aw5ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1kg416a</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>so sparklyyyyy</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bhyaipnuu5ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1kg3ed6</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Whats with this tiny bit of dead skin?</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg3ed6</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1kg38th</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Rainy spring = pink and gray</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg38th</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1kg2k6w</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Dotty</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cb13mezqh5ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1kfs9bd</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>New Favorite Purple</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kfs9bd</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1kgps3m</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>fruit salad</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgps3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1kgouiv</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>a serious Nails for a serious woman</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgouiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1kgo5vu</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>This video doesn’t do my newest Galaxy set justice 🌌</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h2xkl47v8aze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1kgo3uc</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Newbie set. How’d I do?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7dvzz6a8aze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1kgkrxh</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Good chrome isolation</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k7leqw0wc9ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1kghz9q</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Lol😅💀 read caption!</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kghz9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1kgh3m7</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>What do you think of these Studio Ghibli press-ons I made?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e371gom3i8ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1kggyum</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Little buggy press ons I did</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mm9wggfah8ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1kgfrd0</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Newest set as a beginner. What do we think? 🩷</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgfrd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1kgflsp</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Most Recent Set I Did!</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgflsp</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1kgf0h1</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>some shorties</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgf0h1</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1kgeify</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>nails i did in class!</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ja06waa5z7ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1kgdgsc</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>First time doing nails on someone else, any criticism is welcomed</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/450n615kr7ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1kgcbot</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>She prettyyy 💖</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/og9nwuk9j7ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1kgb9ut</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Most complex set yet gaaadayum</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/laqtj98rb7ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1kgaodw</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Nail Art Improvement 2023 vs 2025 :)</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgaodw</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1kg9tkq</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>I accidentally made a chrome bird coming out out of skin</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s429yfx807ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1kfifjm</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Spring nails🌸</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1eijgc0270ze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1kfwojy</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>I'm new and want to learn</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kb36t8o0i3ze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1kg5i60</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>A little aura</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg5i60</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1kg4wya</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Did these press-ons for a friend :)</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg4wya</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1kg3gtk</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Cute lil y2k moment I did last night</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg3gtk</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1kg2dbd</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Tried the soap bubble technique</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lx157kmwf5ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1kg0wwg</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>New nails, thoughts?</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kg0wwg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1kg0qzs</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Thoughts on strait man with acrylics ??</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdbjpur2y4ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu May  8 08:12:41 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_11.xlsx
+++ b/data/collected_data/2025_05_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C699"/>
+  <dimension ref="A1:C891"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12316,6 +12316,3270 @@
         </is>
       </c>
     </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1khjgkm</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Red chrome nails got me feelin ✨🧛‍♀️💁‍♀️</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ad3hhdm46ize1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1khjc2e</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Hi everyone! Do these brands work and do they last at least 2 weeks? Thanks for your help</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DJL94KDgOCq/?igsh=ajM1a21sMmhhcjd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1khjah9</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Mom's magic hands made this Black Cherry set happen</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8b80n8m44ize1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1khj6km</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Blue Nails and red aurora chrome</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7v4s8t8t2ize1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1khj6g4</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Perfect nude chrome 💝</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khj6g4</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1khibry</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>A little sloppy but I think I ate</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khibry</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1khi910</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Cherry 🍒❤️what do you think?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psowbvfrrhze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1khhwtv</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Not the best technique but I'm just starting</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9dex2lunhze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1khheaz</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Rainbow Disco Ball</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzi4tdw7ihze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1khhbob</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>PRINCESS NAILS ✨🎀🌸🩷</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4xa1hfghhze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1khgh0v</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Can I fix my nail shape on my own?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khgh0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1khgp5k</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Nail Tech Never Misses!</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khgp5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1khgnxm</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Did I go too simple?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khgnxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1khgnva</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>I started drawing with an universal liner , what do u think? 😁✨</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khgnva</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1khgidh</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Red vampy cat eye</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d93qijh39hze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1khgcbc</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>got these nails done in Sao Paulo</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8tfdc7e7hze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1khg7kg</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Red Magnetic Cat Eye and Gold Lace</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nq0bjl6k5hze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1khg6cl</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>did my first press on nails today and accidentally painted everything upside down 🥲</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khg6cl</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1khfyny</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>She said she wants some EDC Vegas nails. This what I came up with. What y’all think ?</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khfyny</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1kh9tfm</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>@ ex nail biters/pickers: how long did it take for your nail bed to become normal (did it ever become truly normal?)</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kh9tfm/ex_nail_biterspickers_how_long_did_it_take_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1khaj3q</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Divets on sides of free edge?</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydwtkj3rrfze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1khchs0</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Did these on myself today, I am very proud🥰</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/raorwo288gze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1khfgcd</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>It’s been like a year since i’ve had my claws and i missed them so much 🖤</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9snkw861zgze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1khfdil</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Natural nails (been growing them out since February)</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/96oixyjaygze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1khelyr</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Gel X nails won’t stay on</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khelyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1khasdp</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Am I overreacting?</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ntn00hutfze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1khaag5</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Help me pick a shade of pink should</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pj1jy40upfze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1khf83w</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>nitrile glove brand recommendation?</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1khf83w/nitrile_glove_brand_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1khf43p</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Russian Manicure &gt;</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khf43p</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1kheiym</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Recent nails</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kheiym</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1khe67y</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Beach vacay nails!</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khe67y</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1khe3u7</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Daughter does my nails sometimes</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2tuxybnmgze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1khdtmw</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>What are these white markings?</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/owp1jrf2kgze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1khdlgl</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Help choosing shape for nails!</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khdlgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1khcwa7</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>chrome nails.. yay or nay?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vynguwzrbgze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1khc7n9</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Sea inspire nails (plus the rough draft I showed my tech)</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khc7n9</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1khcq2r</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>kiss salon xtend</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5e8zi49agze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1khckap</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>tried that powder color today</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1srztb2u8gze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1khc035</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Growing out french manicure - feeling satisfied.</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khc035</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1khbpvl</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>jumped on the wagon</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khbpvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1khbgif</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Spring into some black nails</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mff5m12czfze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1khb5ov</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Natural nails with acrylic overlays and isolated chrome</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knrcyh1uwfze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1khb11x</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>I’m turning 30 this weekend and wanted to do something fun but now I’m worried this look is a little too young for me? I usually do very neutral colors.</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kw58utisvfze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1khamc6</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>So these gel nails seem to be sticking up or am I imagining it?</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pyoyvfigsfze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1khagnu</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Is a new design simple to fix on gel X</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5iz6bg7rfze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1khaeka</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Strawberry season 🍓</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whdqqx3rqfze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1kh9avt</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Coquette nails</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6hg0p66ifze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1kh92wg</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Red Cat Eye 😻</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh92wg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1kh8go4</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>The colors glow in the dark!</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04ra9aj0cfze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1kh8g18</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Just got my nails done today! Butterfly wings!!! 💖🦋🥰</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh8g18</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1kh7mb5</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Thoughts on these (my work)</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vihm6e5v5fze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1kh7c1w</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>New set for may</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh7c1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1kh6k7p</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Advice on work drama</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mikx2r8yeze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1kh5yu4</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Help - what is going on with my nails? I consistently get gel x but my nail tech just actually declined to do my nails… i work in a club where i have to have them done so i dont know what to do. Is it an infection? My nails started getting like this in the last year and im at a loss. Help :(</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh5yu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1kh5exj</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Kirby nails 💜🩷🩵🌟</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/00ic824ypeze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1kh4va9</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Thumbnail deep split</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh4va9</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1kh4uqg</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Summer vibes</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w07dc82yleze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1kh4r2w</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Gotta catch em all</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kqzd6l6leze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1kh4qsq</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Want do i need to do acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kh4qsq/want_do_i_need_to_do_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1kh4pv9</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Oh, and they glow!</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/glapthfvkeze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1kh4a0i</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Loving this stained glass look!</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh4a0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1kh49zg</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>🪩Disco effect🪩(swipe&gt;)</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh49zg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1kh46tc</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Looking for advice on how to get super hard gel nails</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kh46tc/looking_for_advice_on_how_to_get_super_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1kh3zxj</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Diy chrome nails for the first time and I'm in love🤧</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j68t41qwfeze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1kh3snt</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>New nails!!</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ghumlqtgeeze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1kh3mps</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Not perfect at all but I'm happy with it</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0uj0xbadeze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1kh3lvr</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Is this a normal speed for them to grow?? It makes them so expensive</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh3lvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1kh3kxl</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>birthday nails</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ingk4k9yceze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1kh2lu7</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Can I get a gel manicure with ripped cuticles?</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kh2lu7/can_i_get_a_gel_manicure_with_ripped_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1kh39ms</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>press on nail suggestions?</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kh39ms/press_on_nail_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1kh35gc</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>This set I did yesterday, quite happy with how it turned out!</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jstlh6pw9eze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1kh318v</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>New set first in a decade, is this normal?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh318v</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1kh2oo4</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>☀️☀️☀️☀️</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqcohqgk6eze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1kgvj0s</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Hallmarks of a good salon/nail tech?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgvj0s/hallmarks_of_a_good_salonnail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1kgz1k6</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>What do I need to start making my own press on sets?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgz1k6/what_do_i_need_to_start_making_my_own_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1kh1h8e</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>How to get this milky blue? Inspo @ Azul Gonzalez on Pinterest</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh1h8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1kh1ejf</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>aura nails</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh1ejf</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1kh23kw</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Vacay nails - guess where I am going!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gp0hsnf2eze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1kh1swu</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Are nails really breaking the bank for you ladies?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kh1swu/are_nails_really_breaking_the_bank_for_you_ladies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1kh1sm8</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Chrome polish ✨️</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh1sm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1kh17bp</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Fresh look</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bn6cml2zvdze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1kh14mq</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>My first set for summer 💕</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh14mq</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1kh0100</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Matched my nails to my swim top</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2f22khkndze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1kgzzlv</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Saw Sinners and felt like I needed to go red</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2hyr9pandze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1kgzri3</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Birthday nails!! What do you think? 🥹</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgzri3</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1kgzowg</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>30 Days of Nails - Day 3 - Country Western 🌵🏜️</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m01x7379kdze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1kgzh9o</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Gel builder</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgzh9o/gel_builder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1kgzaic</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>So obsessed with the textures and colors of this set!</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgzaic</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1kgw6gt</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Who else felt it when watching Kim K lose a nail on the met gala red carpet?</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgw6gt/who_else_felt_it_when_watching_kim_k_lose_a_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1kgyxfg</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Nail shape help!</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pno890njfdze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1kgyvw5</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Hair caught in gel/dip after 1 WK growth</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phmb11n8fdze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1kgyq9i</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>BF picked my nails and they’re so cute! 🫶🏻💕🌸</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgyq9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1kgyo9j</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>New vacation set 💙</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yruv0oonddze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1kgybm8</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Gimme butter by DND is just 😍</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ox6630sxadze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1kgybdr</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>My new nails ☺️🥰</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgybdr</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1kgxi8z</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Glazed French!</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjx6ngyj4dze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1kgx7if</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Taking out contact lenses with long nails</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kgx7if/taking_out_contact_lenses_with_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1kgx3tm</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Is this blue any good? My friends said it looked like ink.</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgx3tm</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1kgwn2u</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>2 questions from a newbie who’s never had their nails done professionally</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c20115tdxcze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1kgwmn1</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Pretty 😍</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oiv6fvq9xcze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1khh5tm</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Something Else</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khh5tm</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1khggav</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>How do you remove your contacts with long nails? 😂</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1khggav/how_do_you_remove_your_contacts_with_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1khgbuf</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Clionadh shipping?</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khgbuf</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1khgb7k</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Mind the lighting, it was raining outside</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khgb7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1khga1y</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>LBOH and AI</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khga1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1khg93w</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Product rave review: Essie To The Rescue</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khg93w</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1khg8p9</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Copper &amp; Sapphire</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khg8p9</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1khffy9</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Trash run at work... quick break to take nail pics</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khffy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1khfexi</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Ordered Angel from Zoya, but I think this might be a mislabel</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khfexi</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1khf0sy</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Gel polish allergy?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9tcna5p0vgze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1khev2t</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Which direction do you paint details?</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khev2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1khetk5</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>can i store acetone sideways?</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1khetk5/can_i_store_acetone_sideways/</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1khes03</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>A Bit Dissatisfied</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d2vdcygtsgze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1khepm7</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Matchy manis</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ilfujw77sgze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1khegre</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Can I something to stop this damage/is it from acetone?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khegre</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1khdwle</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Cirque raising prices.</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltogrgotkgze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1khdn4g</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Why no, I haven’t been going out of my way to save my nail from one break just to break it again.</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khdn4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1khdesz</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Mooncat’s Garden of Evil 😈</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khdesz</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1khdba3</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Cuticle Oil question - Jojoba oil or not?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1khdba3/cuticle_oil_question_jojoba_oil_or_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1khda20</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>First time wearing Sour Note from Holo Taco</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khda20</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1khcyd9</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Cirque Colors Retail Therapy Comparison</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1khcyd9/cirque_colors_retail_therapy_comparison/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1khcxk6</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Tried something subtle... And honestly, never again 😆</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khcxk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1khcwzg</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>My first mooncat order</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s16h3qnwbgze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1khcdwn</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Crabby claw</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khcdwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1khc9tg</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Any fellow hyper mobile laqueristas?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcfwzpfb6gze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1khbra9</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>lush is so shifty</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7584gw2w1gze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1khb6b8</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Kisses To My X's is unreal</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y2irwyzvwfze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1khb6e8</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>The perfect color for spring into summer ✨</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ewtm5m80xfze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1khaozw</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Mooncat’s Pangea - my first matte!</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khaozw</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1khaeoo</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>The inspiration and the execution</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khaeoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1kha6iw</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Favorite chrome-like polishes?</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kha6iw/favorite_chromelike_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1kh2old</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Mooncat Magnet</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kh2old/mooncat_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1kh9aqj</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>bad set of acrylics RUINED my nails health and the skin around them</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bh693235ifze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1kh95vu</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Looking for a dupe of OPI Madam President</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh95vu</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1kh8vsc</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Fool's Paradise</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dzae2zf1ffze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1kh895i</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Tokyo💜💙</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh895i</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1kh7y97</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Cirque Rose Jelly:  Experiences? Thoughts?</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh7y97</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1kh7rng</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>2010 called, she loves my nails ;D</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh7rng</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1kh7a8b</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Springy glitter ✨</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh7a8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1kh75g8</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Any 10 free reds that actually look like this?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh75g8</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1kh6f3e</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Mermaid Franken-mani 🧜🏼‍♀️🌊</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh6f3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1kh5xbn</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>olive oil nails :)</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh5xbn</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1kh5oe7</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>3rd day with this mani and I finally like how it looks</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh5oe7</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1kh5kjx</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Glisten &amp; Glow "Love You to the Moon and Back"</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh5kjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1kh4k5l</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Dimension Nails is closing on the 30th of June</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh4k5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1kh49jg</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Failed miserably at duping ILNP amber</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1grldfcmheze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1kh3ww4</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Thoughts on Polish Me Silly?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kh3ww4/thoughts_on_polish_me_silly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1kh3nun</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Born Ugly vs Treetop</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh3nun</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1kh2xh8</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Eerie Silence April PPU</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh2xh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1kh2x57</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Pastel rainbow for spring 🌈</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h75qhtx88eze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1kh2a7o</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Double magnet trick troubleshooting</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh2a7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1kh2a4d</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Nymph</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh2a4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1kh27ya</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Tell The Devil I got that Purple Skunk</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh27ya</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1kh1nrt</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Help with perpetual nail split?</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efrmb859zdze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1kh16vd</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>thought I duped myself…</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh16vd</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1kh0yfm</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>First try at a gradient nail for spring 🌸</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh0yfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1kh0tpf</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Some distinguished lil bees 🐝</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81ib2j3ctdze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1kh0doa</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>💛🤍Breaking the Binary💜🖤</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh0doa</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1kh09hs</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Can I paint this nail?</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh09hs</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1kgzd9o</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Nail help?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgzd9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1kgz191</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>massive clearance on UK website.....</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kgz191/massive_clearance_on_uk_website/</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1kgytnn</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>mooncat cosmic cowboy</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgytnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1kgybkl</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Love the color but not with my skin tone - oh well</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgybkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1kgy06n</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Trying out gradients</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/koerv4li8dze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1kgxwyn</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>What is a finish that you love as a manicure, but absolutely can't stand as a pedicure?</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kgxwyn/what_is_a_finish_that_you_love_as_a_manicure_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1kgxpy4</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Come Again✨️</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgxpy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1kgxkyh</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>My most “out there” manicure yet!</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgxkyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1kgxfoc</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Women Through The Ages</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgxfoc</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1kguvwc</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Moonshine Mani</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kguvwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1kguqrh</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Flower child, for spring? Groundbreaking</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kguqrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1kglzbh</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Anyone know of a similar polish? I regret not buying before it sold out.</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tsg4cjvxn9ze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1kgrkdz</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Top coat that doesn’t shrink?</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kgrkdz/top_coat_that_doesnt_shrink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1kgrkt8</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Essie Glossamer Garments</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hiwm348ccbze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1kgtrtp</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Cuticula Subscription Monthly Box</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kgtrtp/cuticula_subscription_monthly_box/</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1kgt6tc</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>the first set of gel nails i've ever done!!</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgt6tc</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1kgsyx5</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Cirque Jellies + Spotted</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrhkyferubze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1khhat8</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>I did my nails (on myself) after like 2 months 🤭</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khhat8</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1khgkch</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>New nails I did!</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khgkch</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1khei3j</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Hand painted froggy press ons</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjtv46f8qgze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1khbonv</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>trendy gal</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khbonv</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1khawuq</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>The making of my recent Butterfly Queen nail set!</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/Zf6J4CLkJEk?si=s2pA8q1U5fgyPRcG</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1kh7or2</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Differentiated press on nails for customers</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh7or2</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1kh5utb</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Help with nail art</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqdyg784teze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1kh231x</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>¡¡¡ Only pink !!!</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kh231x/only_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1kh14i5</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Cherry vibes with a wild twist. What do you think of the design? It was a challenge but I loved the result.</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jrlyajevdze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1kh0v4s</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>First press on set</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kh0v4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1kgzbls</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>So obsessed with the textures and colors of this set! My nail artist @nails_emmywynn is truly talented!</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgzbls</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1kgx5df</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Made an order for one of my customers!</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6yl9esoc1dze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1kgx4tl</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Definitely made sure I have nails done for my Paul Mitchell the Nail School tour today! 🥰💅🏼</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ct324ck1dze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1kgvrrt</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>This turned out too perfect 💕</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kgvrrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1kgv77l</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>My more than perfect mani... ❤️</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kgv77l/my_more_than_perfect_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1kgtfno</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Is there gel top coat without blue tint?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kgtfno/is_there_gel_top_coat_without_blue_tint/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri May  9 08:12:20 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_11.xlsx
+++ b/data/collected_data/2025_05_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C891"/>
+  <dimension ref="A1:C1078"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15580,6 +15580,3185 @@
         </is>
       </c>
     </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1kic36n</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>I got my nails done yesterday and am really not vibing with the result :( Should I change them?</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6w8jkgsbpze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1kiaw09</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Bday set🌼🌞</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldwkencyyoze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1kiaucw</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>imPRESS colour FX press ons!</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9xwsyssfxoze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1ki9azw</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Should I ask for a polish change?</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4905szymhoze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1kiaj81</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>HOW do i grow my nails faster</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kiaj81/how_do_i_grow_my_nails_faster/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1ki938w</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Press on artist considered nail techs?</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ki938w/press_on_artist_considered_nail_techs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1ki8r9b</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Even in Arcadia</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vbofw480coze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1ki8ob8</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Is this the cuticle or the proximal nail fold? Should I trim this when doing gel nails?</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2f4cn58boze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1ki6pa6</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Deep Nail Split Repair</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nij2dvz6snze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1ki8amq</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>similar color to opi rosy future in dip/powder?</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ki8amq/similar_color_to_opi_rosy_future_in_dippowder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1ki8htm</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6xwf8mf9oze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1ki7xbs</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Cowboy Carter Nails 💜⭐️</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki7xbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1ki7998</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>My new nails !</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki7998</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1ki72et</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Help! Deep crack/split repair</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9g6zayovnze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1ki6vat</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>something stuck in nail and now nail is clear??</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3xyugattnze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1ki6o22</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Sweet &amp; Simple</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fk82bvavrnze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1ki3au9</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Got acrylics for the first time in 3 years :)</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zffe8cdyxmze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1ki3j9w</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Nails lifting after two weeks</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki3j9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1ki5h1z</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Help I need to remove these nails</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ki5h1z/help_i_need_to_remove_these_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1ki62du</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Squoval vs short almond</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki62du</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1ki5bdi</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Best Color</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ki5bdi/best_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1ki5vad</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Mushroom/ Nature Nails 💅🏻✨</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7w2v460eknze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1ki5u1x</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>I thought these press ons were pretty cute! 💚</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki5u1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1ki5fg6</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Summer nails loading.. 🩷💛</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16k38p0bgnze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1ki5djz</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>My attempt at duck nails</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pp12sm0tfnze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1ki5cbn</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Are there any UV Gel Topcoats that don't stain after application?</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ki5cbn/are_there_any_uv_gel_topcoats_that_dont_stain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1ki5amw</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Gel X Black &amp; Classy Stilettos</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki5amw</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1ki58qb</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>I can't wait to use these colors over the next few weeks!</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xbuq5ykenze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1ki58ki</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Almond or square?</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki58ki</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1ki4vxi</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Bridal Shower Nails</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki4vxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1ki4rga</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Aura Nails🩷🤍</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbleqaqcanze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1ki402u</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>I may nailbiter what should I get?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ki402u/i_may_nailbiter_what_should_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1ki3uh2</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>can't keep gel polish on?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ki3uh2/cant_keep_gel_polish_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1ki4fux</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>These are my boyfriends nails. Life is so unfair.</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqzmwiij7nze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1ki485h</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>My 9 year old sister made this press on set. How did she do?</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki485h</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1ki42g7</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Fill in time</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3rnz6ma4nze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1ki3yqa</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Gold glitter GelX set I did on myself!</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jgdby99f3nze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1ki3uy8</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Deliciously glazed 🍩</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0pbn3kj2nze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1ki3ujo</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Just proud</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki3ujo</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1ki3rj1</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>First time at a salon in a while…</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki3rj1</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1ki395p</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Why does it h*rt so bad???</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ki395p/why_does_it_hrt_so_bad/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1ki340o</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>birthday nails! pink ombre x chrome x hard gel 💖</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki340o</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1ki2x2p</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Birthday Nails!</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki2x2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1ki2m6a</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbn62spdsmze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1ki2kze</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>New spring daisies 🌼</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki2kze</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1ki2h6e</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Can not stop staring at this set I did !!!</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/quag94marmze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1ki26bd</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Cat eye effect and free handed butterfly with gold chrome borders 🦋</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjuiw61yomze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1ki24vb</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>2nd Try At Cateye Designs</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2uuwzo4nomze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1ki21j7</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Bonitas</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxi26g9ynmze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1ki1otq</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>2010 galaxy pants</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki1otq</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1ki1oh9</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Anxiety ease request?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ki1oh9/anxiety_ease_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1ki180z</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>please help</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iiutd3qqhmze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1ki1iv4</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Blue it is!</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fd21db3zjmze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1ki1hor</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Can you tell that these are press ons?</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fugtw1uqjmze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1ki1dqi</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>love the deep red shine on my new nails</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09r9prntimze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1ki1bsu</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Painted my nails! 🧿 Got a lil wild with the layering and I regret my middle finger choice 😂</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t237cmciimze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1ki126d</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Gel extensions from Amazon.</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w970j3yjgmze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1khzpcm</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>What do i ask for at salon?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khzpcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1ki066x</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>DND Lava #759 ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62t78xex9mze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1ki01bp</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Testing Color Changing Gel Polish</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki01bp</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1khzzh7</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Getting my nails done soon</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vw7bwgdk8mze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1khzy2d</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Love fresh nails ❤️</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khzy2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1khznus</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Nails feel sticky/tacky?</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1khznus/nails_feel_stickytacky/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1khzwrc</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Giving club penguin water dojo☁️🌬 🌊</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khzwrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1khztoc</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>It’s really spicy 🌶️ orange (!)</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83915pme7mze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1khzrse</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>What do you think</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xlmwu317mze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1khzdr4</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>should i go get a polish change?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khzdr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1khz2i4</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Cotton Candy Cat Eye</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c31g8t9t1mze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1khyv7z</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Fear of developing an allergy</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1khyv7z/fear_of_developing_an_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1khyq95</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Is it time for a refill?</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khyq95</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1khymth</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Slowly been working my way up to talons 🖤</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ytdpk5pylze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1khyf05</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Press ons too large or small?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khyf05</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1khya5v</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>How do we feel about long nails!?</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2re31g44wlze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1khy29v</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>allergic reaction &amp; gel questions: did these with a beetles gel polish &amp; acrylic press on uv cure, need new stuff?!</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udfolmwkulze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1khy1na</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Cat nail help!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmtlkjagulze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1khy58u</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Kitty nails🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khy58u</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1khy57b</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Fancied super bright this month!</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hj0ej696vlze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1khxrk6</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Did my own gel!</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khxrk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1khxpj4</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Color advice</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khxpj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1khxhfv</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Got bored...</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqpwjaaeqlze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1khxghv</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Spring Nails are Always the Best</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hf81l9l7qlze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1khx74p</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>First time using builder gel!</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khx74p</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1khwtln</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Absolutely spring vibe in my new work 🌸✨</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khwtln</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1khwilm</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Calling all Glam-mas</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khwilm</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1khw564</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Nail book!</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nv166eoxglze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1khvw5z</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Give time for nails to breathe- myth or not?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1khvw5z/give_time_for_nails_to_breathe_myth_or_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1khvgrm</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Why do my nails always look like this when I grow them out?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uf75bi42clze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1khvotx</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>My bridal nails!!!</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khvotx</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1khvaug</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>birthday nails! 🍰🍓</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khvaug</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1khv520</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Going to a wedding this weekend! @v.rnish</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khv520</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1khv2bq</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Fake nails for kids?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1khv2bq/fake_nails_for_kids/</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1khufkl</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Bird beak nails. 🐦💅🏻</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khufkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1khuzz7</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>I made these press ons!</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/873rp0nm8lze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1khumfc</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Holo Taco Missed Shift!</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khumfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1khum88</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Crazy set I did for my bestie for a Japan trip! The CD spins!!</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khum88</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1khu4rq</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Any Tips or advice? 🫠</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khu4rq</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1khtya2</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>New kitty claws 🐈‍⬛✨</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2cqqic651lze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1khttc1</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Ruby gemstone nails 💅</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8t229ab40lze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1khtjd9</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Refillable nail oil pens</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1khtjd9/refillable_nail_oil_pens/</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1khoswa</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Troubleshooting UV allergy?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1khoswa/troubleshooting_uv_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1kid5n0</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>ILNP-High Voltage. Kind of obsessed 💜💜</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kid5n0</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1kicwdw</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Will Cirque Colors restock?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kicwdw/will_cirque_colors_restock/</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1kibje8</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Got my nails done in Tokyo!</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bup7u8pk6pze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1kib5uj</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>any swimmers out there?</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhxnpxi52pze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1kia6kl</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>[Doom Loop Naturals] Breakfast at the End of Time</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kia6kl</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1kia2s2</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Getting the hang of layering ✨</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kia2s2</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1kia0yh</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>First Holo Taco -- Floor is Guava</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0cdw156apoze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1ki9q9p</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Vintage Sally Hansen matches my blue kyanite ring! 💙</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki9q9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1ki9h5c</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Why can't I buy OPI gel polish?</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ki9h5c/why_cant_i_buy_opi_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1ki8z1a</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Is this the cuticle or the proximal nail fold? Should I trim this when doing gel nails?</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h28sv2d8eoze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1ki8n98</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Even in Arcadia</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pza6orjwaoze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1ki8igg</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>mooncat castle of cobwebs 😳</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlcz7qrl9oze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1ki8eqh</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Polishes that makes you look super tan or gives good contrast against brown skin</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ki8eqh/polishes_that_makes_you_look_super_tan_or_gives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1ki7s50</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Desktop manicure caddy/organizer?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ki7s50/desktop_manicure_caddyorganizer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1ki78y4</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Can anyone help me find something for a friend who went through chemo?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ki78y4/can_anyone_help_me_find_something_for_a_friend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1ki6uku</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Simple, but I love this color combo</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki6uku</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1ki699o</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>I took this for a photography class and my classmates gassed me up about my nails!</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9c0m74t9nnze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1ki667b</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>this polish looks like copper foil</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki667b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1ki65bq</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Little Star</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki65bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1ki5r3e</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>spring stickers!</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxrzmh3bjnze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1ki5kg9</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Channeling my inner Lisa Frank Bog Witch today</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki5kg9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1ki5efl</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>LBoH responded, sugar bubbles celebration plate removed</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ki5efl/lboh_responded_sugar_bubbles_celebration_plate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1ki4b52</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>my life as a shrimp</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1epl4hdd6nze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1ki3y5i</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>GLITTERRRRRRR:DDDD</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki3y5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1ki3ske</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Fellow laqueristas, how far do we take this?</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqfx6vw02nze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1ki3pfj</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Kintsugi inspired mani 😂😭</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vf4rmzda1nze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1ki3gyw</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>What is this polish?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki3gyw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1ki2ife</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Help! How should I go about shaping nails like these?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki2ife</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1ki38is</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>I am curious if this look ok? New to nails.</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ki38is/i_am_curious_if_this_look_ok_new_to_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1ki2jip</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>when life is falling apart but the mani is persevering</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki2jip</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1ki1jef</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Anyone have swatch/mani pics of Sparkle from Phoenix Indie?</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1uqwn8utjmze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1ki1dwq</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>My favorite prugly</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2e8u7dyyimze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1ki1c1a</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Will Glampire by Sassy Sauce ever come back?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ki1c1a/will_glampire_by_sassy_sauce_ever_come_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1ki0y9a</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Opals</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ki7oxoojfmze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1ki0l7r</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Emily de molly sheer tint compared to Cracked and Cirque</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ki0l7r/emily_de_molly_sheer_tint_compared_to_cracked_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1ki091r</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Polish Me Silly’s Lollipop Glow</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki091r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1khzr10</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Are there any Kbshimmer 1st purchase promo codes or referral codes? Any type of sale codes honestly 😅 the shipping is putting me over budget here</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1khzr10/are_there_any_kbshimmer_1st_purchase_promo_codes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1khz7lj</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Newbie Before &amp; After</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khz7lj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1khywj3</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Huge thanks to the redditor who destashed this to me! Cellular by Rogue Lacquer from March’s PPU</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khywj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1khynx5</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>KbShimmer How Polarizing</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1khynx5/kbshimmer_how_polarizing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1khq8jo</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>tips to make my nails grow</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/npq9zww79kze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1khyf5l</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Best Neutral Base Coat</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1khyf5l/best_neutral_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1khy8iq</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>i hate my natural nail shape</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5k9ig9msvlze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1khxyqp</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Longest Mani Ever :)</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4enkd6tttlze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1khx9xx</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Dam Polish’s Pro Choice AF</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tlx7hagwolze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1khx3qz</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Not Today Satan!</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khx3qz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1khwoeu</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>F for the Fallen</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbvge6qpklze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1khwaz5</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>When your polish chips do you redo the whole nail or just fill in the spot??</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2nteig2ilze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1khvzct</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Juicy Thermals</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khvzct</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1khvhap</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Mooncat Quicksand’s Embrace</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aw8pb706clze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1khvhc3</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Going away to college in the fall. What/how many polishes should I bring? What would you bring?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1khvhc3/going_away_to_college_in_the_fall_whathow_many/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1khv6fu</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>RIP Dimension Nails :(</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khv6fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1khv0bg</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Is glam polish good despite the brushes? What’s your favorite one?</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1khv0bg/is_glam_polish_good_despite_the_brushes_whats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1khuvsi</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>my magnet setup for effortless cat-eye!</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khuvsi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1khulia</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>New Holo Taco Disco Cowboy Polishes 🤠</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khulia</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1khuihv</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>L.A. Colors polish brush too big....</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1khuihv/la_colors_polish_brush_too_big/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1khugeq</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Any recs for a polish like this?</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awt6voas4lze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1khuamj</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Thank you Laqueristas!!</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khuamj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1khu47p</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>If They Only Knew the You that We Know</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khu47p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1khu0tq</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Filed down my claws, felt neutered, turned my nails into strawberry candies!</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khu0tq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1khtt69</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Alchemy lacquers europe?</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1khtt69/alchemy_lacquers_europe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1khtrxs</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>“Teeny Bopper” from Broken Pixel Polish</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khtrxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1khtamv</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>alternate uses for gel</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1khtamv/alternate_uses_for_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1khsyof</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>new neon fan</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khsyof</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1khsbek</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>la petite mort has my heart 🦋✨🌷</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khs9ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1khrukn</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>anyone else enjoy matching their nails to the weather? 🌩️</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khrukn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1khr8py</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Neon rainbow?</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khr8py</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1khqm2j</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>one month of growth!</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khqm2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1khqiaw</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>First time using Mooncat!</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9j69q40fbkze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1khq4f9</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Seasonally Inappropriate 🍁</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khq4f9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1khq0au</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Polish Has Helped in Stressful Times</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khq0au</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1khpqns</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Do you take your nail polish with you on vacation?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1khpqns/do_you_take_your_nail_polish_with_you_on_vacation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1khpm08</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Well this was a pleasant surprise</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khpm08</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1khpgal</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>💙🩵</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khpgal</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1khowgx</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>What’s a polish that’ll help me get this look that isn’t gel?</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khowgx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1khdjkv</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Shout out to all my mobility impaired laqueristas !! ♿️💅</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxy6o0nihgze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1khnyjp</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Downside to getting a fill?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1khnyjp/downside_to_getting_a_fill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1kicgl5</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Creating syrup gels at home</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kicgl5/creating_syrup_gels_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1ki79pi</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Ducky Nails</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki79pi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1ki0jwq</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Aargh! Need help identifying this technique.</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ki0jwq/aargh_need_help_identifying_this_technique/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1ki08gw</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Cowgirl Up 🐮</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ki08gw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1ki059w</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Mary &amp; Max inspired set</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/buhrh1ul9mze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1khk0c5</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>The are like little sun catchers</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0liwcztxcize1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1khoox0</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Pink with leopard accent</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khoox0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1khq4w8</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Diy Gel x, any tips?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khq4w8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1khpnfm</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Is this nailshape achievable on natural nails?</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khpnfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1khmwt9</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>i cant pick what design i want</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1khmwt9</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat May 10 08:10:32 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_11.xlsx
+++ b/data/collected_data/2025_05_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1078"/>
+  <dimension ref="A1:C1268"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18759,6 +18759,3236 @@
         </is>
       </c>
     </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1kj549c</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Spring set I did on myself!</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kj549c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1kj4q55</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>First time I've ever gone for a colour like this, wanted something classy, simple but pretty! 🥰</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ht4cfnbxqwze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1kj4dhi</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Some of my nails over the last 1.5 years</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kj4dhi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1kj40r6</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>What has happened to my nails?</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjfu4f1aiwze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1kj2zdk</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Micro painting technique with watercolor</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbobupqt5wze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1kj2myi</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Best set I’ve done so far</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kj2myi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1kj29rc</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>blue + orange</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kj29rc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1kj23s4</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>press ons</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kj23s4/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1kj1zjq</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Tips on learning</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kj1zjq/tips_on_learning/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1kj1sac</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Discovered I’m only allergic to coloured gel polish but not base and top.</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kj1sac/discovered_im_only_allergic_to_coloured_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1kj1ijw</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>the subtlest french ever</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kj1ijw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1kj1i38</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>(OP: xjvzaex) how can this color be achieved</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sg7lj3kepvze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1kj1hyu</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Best way to fix a bend in a nail?</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kj1hyu/best_way_to_fix_a_bend_in_a_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1kj1g7q</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>HIM &amp; Mojo Jojo</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/euefj7zwovze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1kj13cs</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Any recommendations for a nail drill?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kj13cs/any_recommendations_for_a_nail_drill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1kizpau</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Fun set I did on myself!</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjtgasp37vze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1kj0f5g</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Not copy paste but still loved this set</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kj0f5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1kj06ca</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>🍋🍋Treated myself to a cute set for my first Mother’s Day</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jm2m5o2vbvze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1kizsii</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Cala Posh Dreams Press-On</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qpaehl508vze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1kizmz9</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Does it look to sharp or just fine?</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kizmz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1kio8fu</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Splitting nails (?)</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kio8fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1kix7h4</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kix7h4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1kiyig8</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Fresh set vs. old set</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiyig8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1kiyn1p</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiyn1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1kiwca8</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Can I still use nail polish?</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ms1xvilnbuze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1kiwbij</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Nails lifting after two weeks.</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kiwbij/nails_lifting_after_two_weeks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1kitlr7</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Help Needed After Russian Manicure</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kitlr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1kite59</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Are my nails crooked? How do I stop this from happening?</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kite59</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1kium3b</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Pearls, 3D bows and shiny details. 🎀</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kium3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1kivfdh</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Got chrome for the first time</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kivfdh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1kizbgz</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Blush mani</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yr2ylupe3vze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1kiz6ar</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Nail tip recommendations?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kiz6ar/nail_tip_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1kiz0h1</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>My wedding nails. ❤️</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiz0h1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1kiyn2l</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Brittle nails</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kiyn2l/brittle_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1kiymq3</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Quick lil set for tn</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fcyvrasiwuze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1kiyko3</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>boss, im tired 😭</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngvl7w54wuze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1kiyi5g</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Tips for getting used to longer nails?💜</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jobkuz6gvuze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1kiybiv</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Joining the fruit nail trend</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiybiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1kixtie</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>First ever attempt at fruit/citrus nails 🍊🍋</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kixtie</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1kixehi</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Low key obsessed with my Tech</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fg5ye9g5luze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1kiwrqh</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>This is Me taking a "risk"</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiwrqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1kiwlns</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>I can’t get the dirt out from under my nails.</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiwlns</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1kiwkyk</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Almond</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2l24y0uduze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1kiwhnp</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>My new extra long set</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiwhnp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1kiwfgb</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>What is the best builder gel?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kiwfgb/what_is_the_best_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1kiw81d</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Red nails 💋</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiw81d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1kiw2yh</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Looking for that perfect red</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiw2yh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1kivv0c</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>My vacay nails 🍊🌀</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kivv0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1kiseit</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>I let my boyfriend pick my color and now I’m dying inside</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxnd9ohoftze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1kirv2v</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>My summer sets so far.  Which one you like ?</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kirv2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1kiqfi9</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Kick'n it old school</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiqfi9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1kiuj4h</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>VERY SHORT NAILS IN LIGHT BLUE COLOR</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rz97mnpdwtze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1kiurz8</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Just hand me the drill</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiurz8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1kitqz9</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Base peeling off after 2 weeks?</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvl59sk0qtze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1kit56m</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Summer is in the air</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgxsk4seltze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1kisvtd</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>My simple nails</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqvwvr6cjtze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1kisocw</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>3 hrs later awesomeness</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kisocw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1kisgz9</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>I love a feminine and boring vibe 🤩</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kisgz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1kisehd</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Some nails i’ve done on my friends as a beginner :))</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kisehd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1kis4cb</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Chrome baby blue</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kis4cb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1kirh32</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Finally had the money for nails after months</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lo2sorr8tze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1kis06n</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>What about nail piercings?🫦🐾</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kis06n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1kirygd</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Happiest I’ve ever been ✨</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kirygd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1kir0xv</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Pearl</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kir0xv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1kir0wc</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Canada folks 📣 looking for a product</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3ohr4v85tze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1kiqvf7</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Some more nails done by my girlfriend!! Love the summer vibe</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiqvf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1kiqr3b</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Fishing lure nails at the aquarium</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiqr3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1kiqr17</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>When your acrylic will NOT come off but you refuse to go to the salon 😭😭😭</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwqnchb63tze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1kiqgh4</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Acceptable or should I ask for a fix?</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiqgh4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1kiqdpb</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Vacation set!</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/op4l1swd0tze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1kiq5xs</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Did by myself - wish I used a pinker nude shade for the French tip nails. THIS TOOK ME 3 HOURS LOL kind of hate them but they’re cute in a messy way</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiq5xs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1kipzsl</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>French cat eye🤌🏻</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgq3g9sdxsze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1kipzfj</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Nail day!</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eh60ajxaxsze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1kipza0</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Boo hoo, these took forever. Pls enjoy</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kipza0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1kipxi4</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Nail day :)</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kipxi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1kipt3i</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Spring nails done, idk if I love or hate them</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kipt3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1kipqnj</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>New Chrome</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kipqnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1kip2g5</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>I need advice!</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kip2g5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1kimxfl</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Tips rubbing off?</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kimxfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1kioyqm</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>My recent nail works! 😍</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kioyqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1kip64e</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Picnic nails on my cousin!!</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kip64e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1kip0m8</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Thoughts? 🩶🤍</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wg965td0qsze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1kinn5f</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Cats and dots</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kinn5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1kioilg</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Nail strengthening tips please</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kioilg/nail_strengthening_tips_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1kiohqa</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Red flower 🌹</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiohqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1kiofnw</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Nail Reformation... I was unfamiliar with your game</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiofnw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1kiodsg</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>There are like 4 different colors!</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzf746jalsze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1kio0h2</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>My attempt at fruit nails trend</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zh3z1ukisze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1kinzkn</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>What am I doing wrong that my soft gel nails look like this after a week 😢</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kinzkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1kinx3w</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>painted my nails based on moon moths (i know its kinda bad, but idc)</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kinx3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1kin3py</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>30 Days of Nails - Day 4 - World Stamps 🗺️🗽🏯</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/443ypepmbsze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1kin2iu</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>I’m becoming obsessed with press-ons</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kin2iu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1kimomx</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Just got my nails done</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thovp0us8sze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1kimmop</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>How can I achieve this?</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h34eylaf8sze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1kimmj2</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Does anyone have a clue why this keeps happening???</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ah7uxc2e8sze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1kimmae</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Nails are orange</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kimmae</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1kimjjk</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>shellac manicure w/ chrome</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kimjjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1kilx9k</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Has anyone switched to press-on?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kilx9k/has_anyone_switched_to_presson/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1kimgb9</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Can’t stop staring at my new set — What do you think?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gozyg647sze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1kim970</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>🦋</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyn5lljo5sze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1kj3wl2</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>If you’re familiar with HoloTaco and Mooncat, could you look at my HT collection and suggest which MC polishes you think I’d love? I’m also open to other brands that are fancy! (USA based)</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xiepy73vgwze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1kj3uot</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Neptune Calling Current Events</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/06023yy8gwze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1kj1rhn</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>What ever happened to virago varnish</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0anwih6svze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1kj1gt9</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Will i ever be able to fix my nails?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kj1gt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1kj1f5k</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Cheap + long-lasting brands? (+ other beginner tips?)</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kj1f5k/cheap_longlasting_brands_other_beginner_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1kj0ycv</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Feelin' Berry Cute 🍓💅</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4x4eu5itjvze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1kj01mu</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Sisters, not twins</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kj01mu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1kizeoe</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>house of hades ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9mzf9e84vze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1kiyrs0</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Dupe request - chartreuse with red/pink shimmer</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiyrs0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1kiy60h</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>my first skittle!</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiy60h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1kixurn</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>It’s not easy being green 😢💚</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kixurn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1kixpkt</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Was never really a blue person</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3trnxjsvnuze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1kiwqzr</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Goblins and Ghoulish Dupe?</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiwqzr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1kiwq3s</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Question about Orly Skinny Dip (teal, slight shimmer)</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kiwq3s/question_about_orly_skinny_dip_teal_slight_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1kiwq1q</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Nailtopia Stitch</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiwq1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1kiwj3k</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Took everyone’s recs yesterday and tried the sheer look myself!</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77woqe9cduze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1kiw83s</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>OPI infinite Shine is a mess for me</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kiw83s/opi_infinite_shine_is_a_mess_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1kiw1ra</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Only one coat needed!</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiw1ra</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1kivxlo</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Duping ILNP Up Above</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kivxlo/duping_ilnp_up_above/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1kivx2o</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>I AM ON MY HANDS AND KNEES WHAT IS THIS POLISH</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kivx2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1kivnru</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Essie’s Congrats ✨ channeling this energy for myself ahead of a big exam!</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kivnru</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1kivb2f</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Devil’s Ivy 🍃</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ok8v3tvq2uze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1kiv8s3</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>A fresh start</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiv8s3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1kiuuku</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Welcoming the lilacs</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiuuku</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1kiul2c</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>can it be saved???</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiul2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1kiuc1d</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Speak to me of nail stamping!</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kiuc1d/speak_to_me_of_nail_stamping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1kiu56c</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Please help- nervous about photos being done for adoption brochure- need to pick nail color</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiu56c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1kitgda</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Dragapult and baby Dreepy's!</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kitgda</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1kitfab</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Finally tried the peely base chrome powder trick!</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kitfab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1kit8q6</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Serpent’s Tongue</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kit8q6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1kisucv</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Flying Pig Nails for the Flying Pig Marathon!</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kisucv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1kis8cg</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Card Trick - Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kis8cg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1kip6fw</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Suncoat Polish?</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kip6fw/suncoat_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1kipxss</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Have been feeling the blues this spring!</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kipxss</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1kiq5bq</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiq5bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1kis22h</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Ok, this is not 💅 exactly, but I was scrolling thru nail swatch feeds, &amp; a ring stack ad popped up. &amp; idky, but I'm now *dying* to deck my hands out like art. I want the polish/blings/rings all of it 😭 does any1 have jewelry brands they love for hand jewelry? W/o breaking the bank?</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kis22h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1kirone</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Little accent moment</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kirone</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1kirm9n</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Grandmacore Nailart</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kirm9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1kiqvyq</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Micro Air Bubbles Driving Me Crazy, Help!</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yfvnznc04tze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1kiqqlg</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>A neon red that hurts the camera</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiqqlg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1kiqc21</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Apocalypse Polish Presents: The Last of Them Collection</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uw9s8t46zsze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1kiq7ji</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Trying out velvet and cat eye</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hhidkrp0zsze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1kiq066</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Some recent sets I've done ✨</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiq066</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1kipm7k</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Has anyone got a comparison swatch between Cirque High Roller and Miami-Dade?</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kipm7k/has_anyone_got_a_comparison_swatch_between_cirque/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1kipaa1</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Had a little helper with my Clionadh order</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8b1yt19zrsze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1kip15p</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>mooncat mermaid bait 🫧</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kip15p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1kiodxq</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>First LynB order and need recommendations!</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kiodxq/first_lynb_order_and_need_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1kio3ww</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Mother’s Day flowers!</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kio3ww</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1kinr67</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Color Request?!</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kinr67</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1kinasz</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>They're the same picture, Cirque</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kinasz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1kimz34</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Glow-in-the-Dark Polish Recs</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kimz34/glowinthedark_polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1kilsda</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Any Peel-Off Basecoats in Canada? (Dam Reflective Glitter Polish Update)</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1t9nat592sze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1kilnlx</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Not sure how to feel about this thermal polish....</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/943l31mh0sze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1killhd</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>New favorite skittle</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1killhd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1kilcfj</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Only highlight of getting an IV in my hand was all the compliments for my nails</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0psvinzyrze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1kil96g</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Gimme all the glitter</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kil96g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1kil8hj</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Mooncat - The Arsonist</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hbn8j216yrze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1kijwfn</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Finally got my hands on Jewel Beetle, and it’s gorg</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kijwfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1kijlkb</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Tariff Casualty - Triple O Polish</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/023loznkkrze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1kijj1i</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>I'm loving this combo 💜❤️</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kijj1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1kijaik</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Was going for terracotta… got leather instead</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kijaik</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1kiiswt</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>i get the hype</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiiswt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1kihre6</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Big Alchemy Lacquer Fan</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kihre6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1ki439w</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Sparkly spring garden nails</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzqzcp7i4nze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1kid7b8</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Finally Back!!</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1rjgsxrrpze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1kig154</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>HELP!!! HOW DO I FIX THIS</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7y2vv64iqqze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1kifrjt</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Looking for builder gel color inspo to match my wedding dress + ring!</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kifrjt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1kie6wl</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Original Barry M sheer strength VS "jelly" sheer strength</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kie6wl/original_barry_m_sheer_strength_vs_jelly_sheer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1kidqpd</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Clionadh haul</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kidqpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1ki6imj</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Looking for a Dupe of this Base Coat - Suggestions?</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9zqftp5nnze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1kj3v60</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Tips for shaping</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hk836degwze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1kj26mb</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>chrome</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xl4xvyswvze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1kj0k5t</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Work I’ve done this week 💕</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/euxhc47sfvze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1kj0iwq</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Today’s work</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hdkyqnqffvze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1kixixx</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>My clients duo ✨</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oc6b720bmuze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1kiwpya</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>This is me taking a risk 🙈</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiwpya</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1kivjgm</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>this weeks nails!</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v87kbivq4uze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1kiuyft</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Bestie and I did a collab on these nail sets for 420!</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiuyft</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1kiupxg</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Pearls, 3D bows, and sparkly details. 🎀</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiupxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1kir947</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Some stuff I’ve done recently (first post on this sub)</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kir947</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1kir2bv</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Pearl</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kir2bv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1kiqiyn</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Going short</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dhodn2g1tze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1kiqeog</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>A little crome initial for each my moms kids for mothers day nails</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjwh60ek0tze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1kiq50g</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Nude florals</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiq50g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1kipkp9</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Our set is done. What do you think?</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ivtdrb7usze1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1kioi3t</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Sets I’ve done this week</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kioi3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1kinmcx</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Cats and dots</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kinmcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1kimvcp</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>First time doing my nails (gel x)</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kimvcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1kifohz</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Any easy DIY nail art ideas for beginners with no tools?</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kifohz/any_easy_diy_nail_art_ideas_for_beginners_with_no/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1kie950</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Aquarium-Inspired Nail Art Ideas 💅🐠✨</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8ehujvj5qze1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun May 11 08:10:34 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_11.xlsx
+++ b/data/collected_data/2025_05_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1268"/>
+  <dimension ref="A1:C1446"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21989,6 +21989,3032 @@
         </is>
       </c>
     </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1kjvpgo</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Crafted with love....by yours truly</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjvpgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1kjvp4e</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Did nail biting cause wider fingertips, or is it natural?</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8a2ct4uy30f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1kjvn4v</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>French with cat eye</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3tg1vfq5y30f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1kjv4fa</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>So shiny!</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zo1dyjztr30f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1kjv2n4</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Shape ok?</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/73bdgv38r30f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1kjuo1g</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>new set</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybun8ghbm30f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1kjunqt</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>I made myself a new set (begginer)</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjunqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1kju0m7</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>I did my friend's birthday nails 🎂🥳</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kju0m7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1kjtoib</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Purple/silver french mani I did</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/427r2spca30f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1kjtn5y</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Maybelline fast gel caramel crush dupe</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kjtn5y/maybelline_fast_gel_caramel_crush_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1kjthrd</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>I FINALLY figured out how to stop my gel from peeling</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjthrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1kjsvoe</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Chrome never gets old.</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jitq7pcxx20f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1kjst3c</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>See through nails</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjst3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1kjspzv</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Help me settle an argument.</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ej3wivwdz20f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1kjspzb</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>New Job nails</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kjspzb/new_job_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1kjsop2</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Cute?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0w2psvzyy20f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1kjsczq</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>I think my nails look gorgeous today!</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/658sdh2iv20f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1kjscyl</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Water color nail polish</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjscyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1kjsa77</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjsa77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1kjrtgm</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>My first attempt at a 3D flower 🥹</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjrtgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1kjrqp2</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>I did another stained glass nail set but this time with cat eye polish 😍✨ what do we think?</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjrqp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1kjpd0d</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>So confused.. what's the best type of fake nail treatment to give me a natural, slightly-extended Mani?</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kjpd0d/so_confused_whats_the_best_type_of_fake_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1kjrh4x</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Crosspost: Has anyone used nail wax while growing out nails?  Any experience with “Just Like Jane”?</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kjrh4x/crosspost_has_anyone_used_nail_wax_while_growing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1kjri0y</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Made these cute nails</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1q0jijwfm20f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1kjrhpg</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Spring is here!</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcnvs9qcm20f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1kjre7n</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Giving this beautiful effect/design a chance ! What do you think?🩵</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jp85popbl20f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1kjre52</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>How are these?</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjre52</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1kjkza3</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Split nail</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0psas7kvw00f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1kjlf4y</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>First time getting nail art</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjlf4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1kjqxb5</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>For My Vegas Trip 😙🍒</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjqxb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1kjpdt8</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Hi is do you tell if you have Ring(s) of fire without removing the nail?</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etutbwlx020f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1kjqlht</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>today’s nails</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjqlht</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1kjqcjk</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>First ever at home GelX</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pw6a033ka20f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1kjq7ax</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Back to the short side</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjq7ax</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1kjq4d4</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Best cat eye polishes?</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kjq4d4/best_cat_eye_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1kjq0go</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Sculptured acrylic nails</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kh05o1m4720f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1kjpwq9</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnj6o4l5620f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1kjpvl0</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Best uv cure gel polish brand for at home?</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kjpvl0/best_uv_cure_gel_polish_brand_for_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1kjpn4e</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>What nail shape looks best on my hands?</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjpn4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1kjmtrz</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>This is why nail salon #s are going down, I wanted to cry</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjmtrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1kjox0h</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>I have a gel polish allergy. Can I still get acrylics and use regular polish?</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kjox0h/i_have_a_gel_polish_allergy_can_i_still_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1kjop79</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>I ordered this gelish color off their website. A week after applying I'm thinking "I would have sworn this was purple". The color in the bottle matches the outside. Why would it do this?</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n37xx4b8u10f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1kjom22</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>In love.</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjom22</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1kjk3v7</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Are these too wide or am I too picky?</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjk3v7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1kjhrdd</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Soap nails will fix my brittle nails?</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0y5y7yf600f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1kjkcup</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Americans, why do you care more about design than quality of nail?</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kjkcup/americans_why_do_you_care_more_about_design_than/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1kjofbe</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Game Day means Nail Day!</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjofbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1kjnt14</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Step by Step for Press-On Nails</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kjnt14/step_by_step_for_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1kjnlyb</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>I think my nails coming off?</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjnlyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1kjng06</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Turquoise Tiger 🐅🦋❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bcux45s9i10f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1kjnd90</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>I loved my manicure, I think it's very elegant 😍💅🏼</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhg0rf0mh10f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1kjmto1</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Yozakura - Cherry Blossoms at Night</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbmrl1ppc10f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1kjmlgu</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Fruit nails update</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjmlgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1kjmlbu</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Certified silly geese 🪿</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1i1o7zgna10f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1kjmgu0</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Are these good for a first time nail (AT HOME) I’m 16 be nice 💔</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mu8ylxri910f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1kjmcdd</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Did a "gardening" themed set for my drag show</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjmcdd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1kjma8a</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Is there something wrong with my nails?</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjma8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1kjm6ts</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Dunkin Nails</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mbcr79b3710f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1kjm4a7</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>advice on improving?</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjm4a7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1kjm49b</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>did my own nails - abstract</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjm49b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1kjlfk8</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>I think my natural nails look fabulous today🩷🌸✨😍</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjlfk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1kjlc24</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Gel polish not lasting as long with builder base</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kjlc24/gel_polish_not_lasting_as_long_with_builder_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1kjl20f</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjl20f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1kjkli4</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Glitter</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42jtzxgrt00f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1kjkjz2</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Vacation nails!</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q89qlt5ft00f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1kjk6hz</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Haven’t done my nails in a while and wanted a bit of everything</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjk6hz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1kjk5mo</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Press on nails I made for myself.</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9581dhw4q00f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1kjjx5n</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>can i file down these little bubbles?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjjx5n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1kjjup4</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjjup4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1kjhp90</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Pink pilates princess theme</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjhp90</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1kjjj9k</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>First press on attempt</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgziis7zk00f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1kjhodv</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Inspo reddit pic from /gallyhill13 vs what I got. Should I get redone?</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjhodv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1kjj9vo</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Advice for cleaning cuticles without cuticle remover</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kjj9vo/advice_for_cleaning_cuticles_without_cuticle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1kjjdsj</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>🧡 ILNP Turbocharged ⚡</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjjdsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1kjj8yr</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Credit to Esthetics by Katie in Nova Scotia. She set me up and I’m ready to go see Avril Lavigne!! 🖤</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufubs4dni00f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1kjj35g</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>She wants everything gold for her Birthday. What you think ?</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcvlp5lbh00f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1kjiocb</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>💙🤍</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7sjh2wq1e00f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1kji8zb</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>What have I done?</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kzc4n3ia00f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1kjhxyr</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Branching out and got a design today. I just love them! 🥰</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjhxyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1kjht56</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Just did a 4 hour nail oil soak in my nitrile gloves</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46t0qbpu600f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1kjhqs8</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>New mani</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijjw473b600f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1kjhk2x</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Can anybody recommend a nail polish (not gel) similar to this?</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjhk2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1kjhmh0</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Fresh Mani</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjhmh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1kjhmco</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>A set to match my wedding ring💜</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjhmco</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1kjgrxr</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Beginner questions</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecilzxbjyzze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1kjghwm</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Trying a new shape. Haven’t had a manicure in 2 months. I feel like a woman again 🥹 2nd pic was my last manicure.</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjghwm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1kjggft</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Question—New nail tech + salon</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kjggft/questionnew_nail_tech_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1kjg1wm</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Clean girl nails, soap nails, lipgloss nails, jelly nails, classy nails… so many names on social media, how would you call them? 💅✨</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zusfp2wszze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1kjfzs6</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Showin' off my shiny white French tips. I absolutely love 'em so much! 🥰😁✨️💕🤍</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8g80qryeszze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1kjfje4</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Sparkly purple nails! Pics don’t do the color justice.</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjfje4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1kjfbia</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>First attempt at chrome, so good!</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjfbia</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1kj3t6t</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Why are my nails like this</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kj3t6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1kjf261</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Lifting in middle of hard gel extensions</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjf261</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1kjd76g</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Why is my dip cracking?</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lb7cu66y5zze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1kjdsde</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Summer Sunset Vibes</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ux5hdpdmazze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1kj7erh</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>3D art + other tings</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kj7erh/3d_art_other_tings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1kjewje</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>3d Gel</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kjewje/3d_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1kjeify</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Color recommendations needed</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kjeify/color_recommendations_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1kje8rs</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Fancy Gloss - Beautiful but Deadly</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kje8rs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1kje1ob</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>I will never surpass the range of nude colors, a lot of elegance✨</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kje1ob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1kjtwja</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Mermaid tail</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjtwja</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1kjslsw</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>2000’s called &amp; they love my nails</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjslsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1kjrsso</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>if you could recommend only one mooncat polish to own, what would it be?</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kjrsso/if_you_could_recommend_only_one_mooncat_polish_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1kjr0dy</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>So confused.. what's the best type of fake nail treatment to give me a natural, slightly-extended Mani?</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kjr0dy/so_confused_whats_the_best_type_of_fake_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1kjplx5</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Apocalypse Polish - Flayer Of Minds (swipe for duck)</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjplx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1kjplkm</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Mooncat Pandemonium - a total stunner</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjplkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1kjpcb9</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>So does anyone else paint their nails better when they’re long?</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kjpcb9/so_does_anyone_else_paint_their_nails_better_when/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1kjn28j</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>DAE intentionally buy similarish polishes just for a skittle?</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kjn28j/dae_intentionally_buy_similarish_polishes_just/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1kjmoh9</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Sea glass copycat</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjmoh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1kjmlm9</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Happy 1-year birthday to my nails!</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jik3s6aqa10f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1kjmcma</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Experimenting with a polarized filter for nail pics</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xmztay9h810f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1kjlsrt</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Mix and Match Nails - Inspired by @5x2.nails on insta</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icn62pep310f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1kjlrsw</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Praise the Dog</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjlrsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1kjl313</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>OPI The Leo-nly One x3, SH IDTC</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjl313</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1kjl2ms</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Tried dotting tool for the first time</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jloxb5pnx00f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1kjkx7i</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Finally made it 😭</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjkx7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1kjktgx</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Optic Bloom🌺🪷</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cjxxgo9jv00f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1kjkjju</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Spring has sprung! 🔥🍓</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjkjju</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1kjk9lx</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Can we talk brushes for a minute?</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kjk9lx/can_we_talk_brushes_for_a_minute/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1kjjsnq</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Just did a 12km mud obstacle race and they survived!!!</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhpzig65n00f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1kjj35y</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Don't judge a polish by its bottle!</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjj35y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1kjj043</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>🧡 ILNP Turbocharged ⚡</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjj043</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1kjisut</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Any other engineers lurking here? I call this shade Loctite 222!</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35p1ahl2f00f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1kjih3h</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Has anyone tried Care and Fix nail concealer or bond treatment to strengthen nails?</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kjih3h/has_anyone_tried_care_and_fix_nail_concealer_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1kjif7t</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Blue creme + green glitter topper</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/BsAd8XO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1kjhj12</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Having way too much fun duping colors</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tj2bb30h400f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1kjhdiu</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Another request for help identifying a lacquer</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kjhdiu/another_request_for_help_identifying_a_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1kjhdfv</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>All Fired Up</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjhdfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1kjh97c</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>First attempt at stamping</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjh97c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1kjgrnq</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>😭😭</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1ciizigyzze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1kjgb01</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Fierce Mojo never disappoints!</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l4km36fuuzze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1kjg1j8</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Brinkley - Zoya 💕</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjg1j8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1kjfp5k</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Heard some of you freaks are into unicorn pee</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjfp5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1kjfmlm</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Stamping polish in tariff world</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kjfmlm/stamping_polish_in_tariff_world/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1kjfdho</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>I feel like a sparkly unicorn ✨️</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kfkka75gnzze1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1kjfars</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Accidentally matched my medicine</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4eh1m9mumzze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1kjf47f</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Sunny Day Sunflowers 🌻</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zb3ohidlzze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1kje90w</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Fancy Gloss - Beautiful but Deadly</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kje90w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1kjd7h8</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Essie - Liquorish on natural nails</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2l9tbqr06zze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1kjd1dc</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Confused if my nails need nail strengtheners or not</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kjd1dc/confused_if_my_nails_need_nail_strengtheners_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1kjd098</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Glossy or matte?</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjd098</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1kjczux</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Hot tip for my fellow chronic cuticle flooders:</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8azwicb4zze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1kjcuav</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>What are almond nails supposed to look like from the side? Can i do almond with my nails?</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjcuav</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1kjckas</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Hypermobile laquristas: let’s see your cursed mani poses!</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjckas</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1kjcfhq</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Mother's day mani</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hvfspuqzyze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1kjc1ta</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>wonky polka dots + birds 🐦🪹</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjc1ta</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1kjbtrm</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Ombre 2.0, glittery boogaloo</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjbtrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1kj8mto</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>How to make my polish last longer?</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kj8mto/how_to_make_my_polish_last_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1kjalwb</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>happy prugly friday</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjalwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1kjalqb</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>And thus begins the great experiment</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjalqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1kjakd3</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>BKL overpours from last release?</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kjakd3/bkl_overpours_from_last_release/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1kjajea</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>you already know which polish this is 🌊</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eg17rzk5kyze1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1kjaa1x</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Such a sucker for a linear holo</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjaa1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1kj9mmc</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>i 🩵 blue polish</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kj9mmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1kj98zm</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>When in doubt, add black flakes</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kj98zm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1kj6ro8</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>HHC Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kj6ro8/hhc_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1kiuv94</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Two color purple skittle</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kiuv94</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1kj60qx</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Dupe or Similar Polish</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kj60qx/dupe_or_similar_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1kj5e8o</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Recommend me multichromes with good durability</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kj5e8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1kjrsr1</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>My first attempt at a 3D flower 🥹</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjrsr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1kjrgbg</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>What are your take on these nails</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o7t5gxsxl20f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1kjre7v</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Daisy 💅</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjre7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1kjq586</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Sparkle butterflies!</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjq586</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1kjph07</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Tips/tricks?</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dwu08rqt120f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1kjogfq</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>My juicy cherry tropical zebra print nail. I sculpted the cherry using 3d gel.</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jk0dc1vtr10f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1kjo8y9</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>My first attempt at pop art.</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjo8y9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1kjo3mo</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>OMGG!!</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzb9llqeo10f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1kjnqmt</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>First Summer Set of The Season</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjnqmt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1kjn22f</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Modeling clay properties that dries hard</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kjn22f/modeling_clay_properties_that_dries_hard/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1kjkaam</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Avril Lavigne ready!! Credit to Katie at Esthetics by Katie in Nova Scotia 💅</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxh55ak6r00f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1kjjyhj</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Concert Nails</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjjyhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1kjiae0</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>I made a tuxedo nail.</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0imirata00f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1kjgd6i</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>Loving the new packaging ✨</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjgd6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1kjeu6s</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>Loon and Trout inspired nails</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjeu6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1kjdm8w</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Where can I find non-AI inspo?</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kjdm8w/where_can_i_find_nonai_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1kjbl5r</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>I made prom nails for my sister’s girlfriend</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjbl5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1kjapox</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Neutral leopard print</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kjapox</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1kj5wtc</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Pink and daisies🌸</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kj5wtc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>